<commit_message>
Added more header columns
</commit_message>
<xml_diff>
--- a/InvoiceBot/SavedInvoiceDataLog.xlsx
+++ b/InvoiceBot/SavedInvoiceDataLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubProjects\New InvoiceProcessing\InvoiceBot2\InvoiceBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044A0278-02B0-4A5F-B805-159ABD194C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1640B3-7770-4AD4-B8E1-D80E2947413E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{71BB526B-92F3-4D18-935F-43566BE0BC34}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71BB526B-92F3-4D18-935F-43566BE0BC34}"/>
   </bookViews>
   <sheets>
     <sheet name="InvoiceLog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>#NO</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Senders Address</t>
   </si>
   <si>
-    <t>Contact Details</t>
-  </si>
-  <si>
     <t>Inv No</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>VAT No</t>
   </si>
   <si>
-    <t>Tax</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -110,31 +104,22 @@
     <t>Total</t>
   </si>
   <si>
-    <t>E.C.C</t>
-  </si>
-  <si>
-    <t>52 Thembigie Johannesburg</t>
-  </si>
-  <si>
-    <t>3rd Floor 22 Dreyer street Sanclare Buiding</t>
-  </si>
-  <si>
-    <t>INFX04062</t>
-  </si>
-  <si>
-    <t>InvF 203430</t>
-  </si>
-  <si>
-    <t>FNB Cheque</t>
-  </si>
-  <si>
-    <t>Imani Olave</t>
-  </si>
-  <si>
-    <t>63 Ivy Rond, Hewkille GA, LISA 31 036</t>
-  </si>
-  <si>
-    <t>ABSA BAMK.</t>
+    <t>Receivers Contact Details</t>
+  </si>
+  <si>
+    <t>Tax No</t>
+  </si>
+  <si>
+    <t>Senders Contact Details</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>VAT %</t>
+  </si>
+  <si>
+    <t>Bank Account Name</t>
   </si>
 </sst>
 </file>
@@ -192,7 +177,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;R&quot;#,##0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -211,11 +196,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -284,32 +281,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}" name="Table1" displayName="Table1" ref="A1:X14" totalsRowShown="0">
-  <autoFilter ref="A1:X14" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}"/>
-  <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{0FA06E5B-1B73-4E73-A44D-1DA293421287}" name="#NO" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}" name="Table1" displayName="Table1" ref="A1:AB14" totalsRowShown="0">
+  <autoFilter ref="A1:AB14" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}"/>
+  <tableColumns count="28">
+    <tableColumn id="1" xr3:uid="{0FA06E5B-1B73-4E73-A44D-1DA293421287}" name="#NO" dataDxfId="27">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{BC2DEE58-FEE2-4400-BFEB-FCEEFF738484}" name="Date" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{84C745BF-B192-406E-AE73-23BE614ABC77}" name="From" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{89ED4BCB-625D-483C-B61D-6C9F06C072FA}" name="Bill To" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{CE912894-973C-4E51-8011-D159986817C4}" name="Senders Address" dataDxfId="19"/>
-    <tableColumn id="24" xr3:uid="{BFE0D837-2C7B-42BD-A16A-DE2CDBF70628}" name="Receivers Address" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{FE59F13E-5A21-47B4-A9EF-18DBAA382ABB}" name="Contact Details" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{87932FF1-0A86-4F0D-9602-C05A18D4337E}" name="Inv No" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{E40660D4-E7F8-4155-BD74-B6079C1EDCB6}" name="Company Vat Reg" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{8E7E6CC3-BCDD-4C4B-AE2F-07C463573FBF}" name="PO No" dataDxfId="14"/>
-    <tableColumn id="23" xr3:uid="{02626E26-D8EF-44B0-9AB4-895DB15E6BAB}" name="VAT No" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{D979257E-475F-4CA9-A983-95369870AF9D}" name="Tax" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{FA249B09-9B2D-4876-8E59-CF7C27DC3832}" name="Description" dataDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{666804AA-1E70-415B-89D1-1A72FAF9F8EB}" name="Service" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{6EC2B118-0451-4EFE-8069-C6E9C3A002C0}" name="Qauntity" dataDxfId="9"/>
-    <tableColumn id="22" xr3:uid="{C05DC58D-14E4-40D2-BE25-405FE840F8AC}" name="Hours" dataDxfId="8"/>
-    <tableColumn id="21" xr3:uid="{C72C2D26-2E38-475A-AE9C-C967A09FC87E}" name="Rate" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{81F48D24-5ACC-4191-A21B-F84B9B5D0FE4}" name="Unit Price" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{634EBF08-2050-471F-A18B-0D975BEC91DC}" name="Price" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{038F4464-83DE-47BF-AAB6-6254BAA84B77}" name="Bank Name" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{BF7433D6-9279-442F-9D38-4A62C589F8B4}" name="Branch Code" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{BC2DEE58-FEE2-4400-BFEB-FCEEFF738484}" name="Date" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{84C745BF-B192-406E-AE73-23BE614ABC77}" name="From" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{89ED4BCB-625D-483C-B61D-6C9F06C072FA}" name="Bill To" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{CE912894-973C-4E51-8011-D159986817C4}" name="Senders Address" dataDxfId="23"/>
+    <tableColumn id="24" xr3:uid="{BFE0D837-2C7B-42BD-A16A-DE2CDBF70628}" name="Receivers Address" dataDxfId="22"/>
+    <tableColumn id="25" xr3:uid="{62DFD726-84D8-495B-B42E-E0A59D973768}" name="Senders Contact Details" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{FE59F13E-5A21-47B4-A9EF-18DBAA382ABB}" name="Receivers Contact Details" dataDxfId="20"/>
+    <tableColumn id="28" xr3:uid="{B1D12C98-53A9-400A-90EC-3EC534830FE4}" name="Email" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{87932FF1-0A86-4F0D-9602-C05A18D4337E}" name="Inv No" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{E40660D4-E7F8-4155-BD74-B6079C1EDCB6}" name="Company Vat Reg" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{8E7E6CC3-BCDD-4C4B-AE2F-07C463573FBF}" name="PO No" dataDxfId="16"/>
+    <tableColumn id="23" xr3:uid="{02626E26-D8EF-44B0-9AB4-895DB15E6BAB}" name="VAT No" dataDxfId="15"/>
+    <tableColumn id="29" xr3:uid="{654A534F-1146-4C55-A284-5C0B5CAF3EB9}" name="VAT %" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{D979257E-475F-4CA9-A983-95369870AF9D}" name="Tax No" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{FA249B09-9B2D-4876-8E59-CF7C27DC3832}" name="Description" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{666804AA-1E70-415B-89D1-1A72FAF9F8EB}" name="Service" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{6EC2B118-0451-4EFE-8069-C6E9C3A002C0}" name="Qauntity" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{C05DC58D-14E4-40D2-BE25-405FE840F8AC}" name="Hours" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{C72C2D26-2E38-475A-AE9C-C967A09FC87E}" name="Rate" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{81F48D24-5ACC-4191-A21B-F84B9B5D0FE4}" name="Unit Price" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{634EBF08-2050-471F-A18B-0D975BEC91DC}" name="Price" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{038F4464-83DE-47BF-AAB6-6254BAA84B77}" name="Bank Name" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{BF7433D6-9279-442F-9D38-4A62C589F8B4}" name="Branch Code" dataDxfId="4"/>
+    <tableColumn id="26" xr3:uid="{B315133D-A01C-4DE4-A4C9-E0FC9A971EA0}" name="Bank Account Name" dataDxfId="3"/>
     <tableColumn id="17" xr3:uid="{339A33EF-F310-4C33-9BA2-332E1474123E}" name="Bank Acc No" dataDxfId="2"/>
     <tableColumn id="18" xr3:uid="{F29665B5-4DF1-44E7-A75D-FA717340214F}" name="Subtotal" dataDxfId="1"/>
     <tableColumn id="19" xr3:uid="{FDD10ED1-DF47-4EC9-AB01-6CA58993EF2F}" name="Total" dataDxfId="0"/>
@@ -635,31 +636,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B17B189-3F58-460C-B125-67DE3543A8D8}">
-  <dimension ref="A1:X14"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="B2:AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.21875" customWidth="1"/>
     <col min="3" max="6" width="104" customWidth="1"/>
-    <col min="7" max="7" width="85.77734375" customWidth="1"/>
-    <col min="8" max="8" width="30.77734375" customWidth="1"/>
-    <col min="9" max="9" width="47.77734375" customWidth="1"/>
-    <col min="10" max="12" width="30.77734375" customWidth="1"/>
-    <col min="13" max="13" width="182.6640625" customWidth="1"/>
-    <col min="14" max="17" width="30.77734375" customWidth="1"/>
-    <col min="18" max="18" width="104" customWidth="1"/>
-    <col min="19" max="19" width="71.44140625" customWidth="1"/>
-    <col min="20" max="20" width="43.44140625" customWidth="1"/>
-    <col min="21" max="21" width="30.77734375" customWidth="1"/>
-    <col min="22" max="22" width="39.6640625" customWidth="1"/>
-    <col min="23" max="24" width="30.77734375" customWidth="1"/>
+    <col min="7" max="7" width="47.77734375" customWidth="1"/>
+    <col min="8" max="9" width="41.21875" customWidth="1"/>
+    <col min="10" max="10" width="30.77734375" customWidth="1"/>
+    <col min="11" max="11" width="47.77734375" customWidth="1"/>
+    <col min="12" max="15" width="30.77734375" customWidth="1"/>
+    <col min="16" max="16" width="182.6640625" customWidth="1"/>
+    <col min="17" max="20" width="30.77734375" customWidth="1"/>
+    <col min="21" max="21" width="104" customWidth="1"/>
+    <col min="22" max="22" width="71.44140625" customWidth="1"/>
+    <col min="23" max="23" width="43.44140625" customWidth="1"/>
+    <col min="24" max="25" width="30.77734375" customWidth="1"/>
+    <col min="26" max="26" width="39.6640625" customWidth="1"/>
+    <col min="27" max="28" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -679,85 +681,85 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AA1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AB1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f t="shared" ref="A2:A14" si="0">ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="4">
-        <v>44294</v>
-      </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -766,36 +768,28 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2">
-        <v>3000</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1">
-        <v>44893279</v>
-      </c>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -807,23 +801,19 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2">
-        <v>774.45</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1">
-        <v>4079342563</v>
-      </c>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3">
-        <v>785.45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -844,15 +834,19 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -873,15 +867,19 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
       <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -902,15 +900,19 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -931,15 +933,19 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -960,15 +966,19 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
       <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -989,15 +999,19 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
       <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1018,15 +1032,19 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
       <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1047,15 +1065,19 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
       <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1076,15 +1098,19 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
       <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1105,15 +1131,19 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
       <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1134,13 +1164,17 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
       <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added an update excel saved sheet sequence
</commit_message>
<xml_diff>
--- a/InvoiceBot/SavedInvoiceDataLog.xlsx
+++ b/InvoiceBot/SavedInvoiceDataLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubProjects\New InvoiceProcessing\InvoiceBot2\InvoiceBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1640B3-7770-4AD4-B8E1-D80E2947413E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D358149B-5BE1-49A1-B11D-1BB0FD0A6BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71BB526B-92F3-4D18-935F-43566BE0BC34}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>#NO</t>
   </si>
@@ -120,6 +120,45 @@
   </si>
   <si>
     <t>Bank Account Name</t>
+  </si>
+  <si>
+    <t>TechZenith Team</t>
+  </si>
+  <si>
+    <t>Corporetior</t>
+  </si>
+  <si>
+    <t>122 Innovation prive, silicon Valley, Cit 95054</t>
+  </si>
+  <si>
+    <t>438a' Street, Anytown, CA 12345</t>
+  </si>
+  <si>
+    <t>TZS-2023-0001</t>
+  </si>
+  <si>
+    <t>Cand ServerhostingUINcth) Website Designs Dav satware Custanization Searty Aadt</t>
+  </si>
+  <si>
+    <t>2 x1 x 5 x 1</t>
+  </si>
+  <si>
+    <t>R500.00 R 3000.00 R150.00 2500.00</t>
+  </si>
+  <si>
+    <t>21000.00 R3000.00 R750.00 2500.00</t>
+  </si>
+  <si>
+    <t>R5250.00</t>
+  </si>
+  <si>
+    <t>R525250.00</t>
+  </si>
+  <si>
+    <t>12-3456789</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -177,7 +216,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="29">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;R&quot;#,##0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -281,39 +323,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}" name="Table1" displayName="Table1" ref="A1:AB14" totalsRowShown="0">
-  <autoFilter ref="A1:AB14" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}"/>
-  <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{0FA06E5B-1B73-4E73-A44D-1DA293421287}" name="#NO" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}" name="Table1" displayName="Table1" ref="A1:AC14" totalsRowShown="0">
+  <autoFilter ref="A1:AC14" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}"/>
+  <tableColumns count="29">
+    <tableColumn id="1" xr3:uid="{0FA06E5B-1B73-4E73-A44D-1DA293421287}" name="#NO" dataDxfId="28">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{BC2DEE58-FEE2-4400-BFEB-FCEEFF738484}" name="Date" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{84C745BF-B192-406E-AE73-23BE614ABC77}" name="From" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{89ED4BCB-625D-483C-B61D-6C9F06C072FA}" name="Bill To" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{CE912894-973C-4E51-8011-D159986817C4}" name="Senders Address" dataDxfId="23"/>
-    <tableColumn id="24" xr3:uid="{BFE0D837-2C7B-42BD-A16A-DE2CDBF70628}" name="Receivers Address" dataDxfId="22"/>
-    <tableColumn id="25" xr3:uid="{62DFD726-84D8-495B-B42E-E0A59D973768}" name="Senders Contact Details" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{FE59F13E-5A21-47B4-A9EF-18DBAA382ABB}" name="Receivers Contact Details" dataDxfId="20"/>
-    <tableColumn id="28" xr3:uid="{B1D12C98-53A9-400A-90EC-3EC534830FE4}" name="Email" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{87932FF1-0A86-4F0D-9602-C05A18D4337E}" name="Inv No" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{E40660D4-E7F8-4155-BD74-B6079C1EDCB6}" name="Company Vat Reg" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{8E7E6CC3-BCDD-4C4B-AE2F-07C463573FBF}" name="PO No" dataDxfId="16"/>
-    <tableColumn id="23" xr3:uid="{02626E26-D8EF-44B0-9AB4-895DB15E6BAB}" name="VAT No" dataDxfId="15"/>
-    <tableColumn id="29" xr3:uid="{654A534F-1146-4C55-A284-5C0B5CAF3EB9}" name="VAT %" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{D979257E-475F-4CA9-A983-95369870AF9D}" name="Tax No" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{FA249B09-9B2D-4876-8E59-CF7C27DC3832}" name="Description" dataDxfId="12"/>
-    <tableColumn id="20" xr3:uid="{666804AA-1E70-415B-89D1-1A72FAF9F8EB}" name="Service" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{6EC2B118-0451-4EFE-8069-C6E9C3A002C0}" name="Qauntity" dataDxfId="10"/>
-    <tableColumn id="22" xr3:uid="{C05DC58D-14E4-40D2-BE25-405FE840F8AC}" name="Hours" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{C72C2D26-2E38-475A-AE9C-C967A09FC87E}" name="Rate" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{81F48D24-5ACC-4191-A21B-F84B9B5D0FE4}" name="Unit Price" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{634EBF08-2050-471F-A18B-0D975BEC91DC}" name="Price" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{038F4464-83DE-47BF-AAB6-6254BAA84B77}" name="Bank Name" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{BF7433D6-9279-442F-9D38-4A62C589F8B4}" name="Branch Code" dataDxfId="4"/>
-    <tableColumn id="26" xr3:uid="{B315133D-A01C-4DE4-A4C9-E0FC9A971EA0}" name="Bank Account Name" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{339A33EF-F310-4C33-9BA2-332E1474123E}" name="Bank Acc No" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{F29665B5-4DF1-44E7-A75D-FA717340214F}" name="Subtotal" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{FDD10ED1-DF47-4EC9-AB01-6CA58993EF2F}" name="Total" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{BC2DEE58-FEE2-4400-BFEB-FCEEFF738484}" name="Date" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{84C745BF-B192-406E-AE73-23BE614ABC77}" name="From" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{89ED4BCB-625D-483C-B61D-6C9F06C072FA}" name="Bill To" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{CE912894-973C-4E51-8011-D159986817C4}" name="Senders Address" dataDxfId="24"/>
+    <tableColumn id="24" xr3:uid="{BFE0D837-2C7B-42BD-A16A-DE2CDBF70628}" name="Receivers Address" dataDxfId="23"/>
+    <tableColumn id="25" xr3:uid="{62DFD726-84D8-495B-B42E-E0A59D973768}" name="Senders Contact Details" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{FE59F13E-5A21-47B4-A9EF-18DBAA382ABB}" name="Receivers Contact Details" dataDxfId="21"/>
+    <tableColumn id="28" xr3:uid="{B1D12C98-53A9-400A-90EC-3EC534830FE4}" name="Email" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{87932FF1-0A86-4F0D-9602-C05A18D4337E}" name="Inv No" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{E40660D4-E7F8-4155-BD74-B6079C1EDCB6}" name="Company Vat Reg" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{8E7E6CC3-BCDD-4C4B-AE2F-07C463573FBF}" name="PO No" dataDxfId="17"/>
+    <tableColumn id="23" xr3:uid="{02626E26-D8EF-44B0-9AB4-895DB15E6BAB}" name="VAT No" dataDxfId="16"/>
+    <tableColumn id="29" xr3:uid="{654A534F-1146-4C55-A284-5C0B5CAF3EB9}" name="VAT %" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{D979257E-475F-4CA9-A983-95369870AF9D}" name="Tax No" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{FA249B09-9B2D-4876-8E59-CF7C27DC3832}" name="Description" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{666804AA-1E70-415B-89D1-1A72FAF9F8EB}" name="Service" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{6EC2B118-0451-4EFE-8069-C6E9C3A002C0}" name="Qauntity" dataDxfId="11"/>
+    <tableColumn id="22" xr3:uid="{C05DC58D-14E4-40D2-BE25-405FE840F8AC}" name="Hours" dataDxfId="10"/>
+    <tableColumn id="21" xr3:uid="{C72C2D26-2E38-475A-AE9C-C967A09FC87E}" name="Rate" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{81F48D24-5ACC-4191-A21B-F84B9B5D0FE4}" name="Unit Price" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{634EBF08-2050-471F-A18B-0D975BEC91DC}" name="Price" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{038F4464-83DE-47BF-AAB6-6254BAA84B77}" name="Bank Name" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{BF7433D6-9279-442F-9D38-4A62C589F8B4}" name="Branch Code" dataDxfId="5"/>
+    <tableColumn id="26" xr3:uid="{B315133D-A01C-4DE4-A4C9-E0FC9A971EA0}" name="Bank Account Name" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{339A33EF-F310-4C33-9BA2-332E1474123E}" name="Bank Acc No" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{F29665B5-4DF1-44E7-A75D-FA717340214F}" name="Subtotal" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{FDD10ED1-DF47-4EC9-AB01-6CA58993EF2F}" name="Total" dataDxfId="1"/>
+    <tableColumn id="27" xr3:uid="{C4CF3119-1363-46DD-BD38-7474CA48138A}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -636,9 +679,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B17B189-3F58-460C-B125-67DE3543A8D8}">
-  <dimension ref="A1:AB14"/>
+  <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AB2" sqref="B2:AB2"/>
     </sheetView>
   </sheetViews>
@@ -661,7 +704,7 @@
     <col min="27" max="28" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,41 +789,75 @@
       <c r="AB1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f t="shared" ref="A2:A14" si="0">ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="B2" s="4">
+        <v>45000</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="1">
+        <v>199549990</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1234567</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+      <c r="P2" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
+      <c r="R2" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
+      <c r="U2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AA2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -812,8 +889,9 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC3" s="1"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -845,8 +923,9 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC4" s="1"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -878,8 +957,9 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC5" s="1"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -911,8 +991,9 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC6" s="1"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -944,8 +1025,9 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC7" s="1"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -977,8 +1059,9 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC8" s="1"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1010,8 +1093,9 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC9" s="1"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1043,8 +1127,9 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC10" s="1"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1076,8 +1161,9 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC11" s="1"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1109,8 +1195,9 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC12" s="1"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1142,8 +1229,9 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC13" s="1"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1175,6 +1263,7 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
+      <c r="AC14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added another invoice template
</commit_message>
<xml_diff>
--- a/InvoiceBot/SavedInvoiceDataLog.xlsx
+++ b/InvoiceBot/SavedInvoiceDataLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubProjects\New InvoiceProcessing\InvoiceBot2\InvoiceBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D358149B-5BE1-49A1-B11D-1BB0FD0A6BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E3B81A-8BE3-427E-A1A1-A55F3279EBD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71BB526B-92F3-4D18-935F-43566BE0BC34}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>#NO</t>
   </si>
@@ -122,43 +122,25 @@
     <t>Bank Account Name</t>
   </si>
   <si>
-    <t>TechZenith Team</t>
-  </si>
-  <si>
-    <t>Corporetior</t>
-  </si>
-  <si>
-    <t>122 Innovation prive, silicon Valley, Cit 95054</t>
-  </si>
-  <si>
-    <t>438a' Street, Anytown, CA 12345</t>
-  </si>
-  <si>
-    <t>TZS-2023-0001</t>
-  </si>
-  <si>
-    <t>Cand ServerhostingUINcth) Website Designs Dav satware Custanization Searty Aadt</t>
-  </si>
-  <si>
-    <t>2 x1 x 5 x 1</t>
-  </si>
-  <si>
-    <t>R500.00 R 3000.00 R150.00 2500.00</t>
-  </si>
-  <si>
-    <t>21000.00 R3000.00 R750.00 2500.00</t>
-  </si>
-  <si>
-    <t>R5250.00</t>
-  </si>
-  <si>
-    <t>R525250.00</t>
-  </si>
-  <si>
-    <t>12-3456789</t>
-  </si>
-  <si>
-    <t>Column1</t>
+    <t>AntoMoton Motors</t>
+  </si>
+  <si>
+    <t>157 Rodd street, CA, 9456</t>
+  </si>
+  <si>
+    <t>103 Drivency Street, autaille, 9750</t>
+  </si>
+  <si>
+    <t>Hastings Insurance Services Ltd</t>
+  </si>
+  <si>
+    <t>Andre Schoombee</t>
+  </si>
+  <si>
+    <t>INUMB_97122Ud</t>
+  </si>
+  <si>
+    <t>Standard Bank</t>
   </si>
 </sst>
 </file>
@@ -216,10 +198,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;R&quot;#,##0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -323,40 +302,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}" name="Table1" displayName="Table1" ref="A1:AC14" totalsRowShown="0">
-  <autoFilter ref="A1:AC14" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}"/>
-  <tableColumns count="29">
-    <tableColumn id="1" xr3:uid="{0FA06E5B-1B73-4E73-A44D-1DA293421287}" name="#NO" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}" name="Table1" displayName="Table1" ref="A1:AB14" totalsRowShown="0">
+  <autoFilter ref="A1:AB14" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}"/>
+  <tableColumns count="28">
+    <tableColumn id="1" xr3:uid="{0FA06E5B-1B73-4E73-A44D-1DA293421287}" name="#NO" dataDxfId="27">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{BC2DEE58-FEE2-4400-BFEB-FCEEFF738484}" name="Date" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{84C745BF-B192-406E-AE73-23BE614ABC77}" name="From" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{89ED4BCB-625D-483C-B61D-6C9F06C072FA}" name="Bill To" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{CE912894-973C-4E51-8011-D159986817C4}" name="Senders Address" dataDxfId="24"/>
-    <tableColumn id="24" xr3:uid="{BFE0D837-2C7B-42BD-A16A-DE2CDBF70628}" name="Receivers Address" dataDxfId="23"/>
-    <tableColumn id="25" xr3:uid="{62DFD726-84D8-495B-B42E-E0A59D973768}" name="Senders Contact Details" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{FE59F13E-5A21-47B4-A9EF-18DBAA382ABB}" name="Receivers Contact Details" dataDxfId="21"/>
-    <tableColumn id="28" xr3:uid="{B1D12C98-53A9-400A-90EC-3EC534830FE4}" name="Email" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{87932FF1-0A86-4F0D-9602-C05A18D4337E}" name="Inv No" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{E40660D4-E7F8-4155-BD74-B6079C1EDCB6}" name="Company Vat Reg" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{8E7E6CC3-BCDD-4C4B-AE2F-07C463573FBF}" name="PO No" dataDxfId="17"/>
-    <tableColumn id="23" xr3:uid="{02626E26-D8EF-44B0-9AB4-895DB15E6BAB}" name="VAT No" dataDxfId="16"/>
-    <tableColumn id="29" xr3:uid="{654A534F-1146-4C55-A284-5C0B5CAF3EB9}" name="VAT %" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{D979257E-475F-4CA9-A983-95369870AF9D}" name="Tax No" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{FA249B09-9B2D-4876-8E59-CF7C27DC3832}" name="Description" dataDxfId="13"/>
-    <tableColumn id="20" xr3:uid="{666804AA-1E70-415B-89D1-1A72FAF9F8EB}" name="Service" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{6EC2B118-0451-4EFE-8069-C6E9C3A002C0}" name="Qauntity" dataDxfId="11"/>
-    <tableColumn id="22" xr3:uid="{C05DC58D-14E4-40D2-BE25-405FE840F8AC}" name="Hours" dataDxfId="10"/>
-    <tableColumn id="21" xr3:uid="{C72C2D26-2E38-475A-AE9C-C967A09FC87E}" name="Rate" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{81F48D24-5ACC-4191-A21B-F84B9B5D0FE4}" name="Unit Price" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{634EBF08-2050-471F-A18B-0D975BEC91DC}" name="Price" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{038F4464-83DE-47BF-AAB6-6254BAA84B77}" name="Bank Name" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{BF7433D6-9279-442F-9D38-4A62C589F8B4}" name="Branch Code" dataDxfId="5"/>
-    <tableColumn id="26" xr3:uid="{B315133D-A01C-4DE4-A4C9-E0FC9A971EA0}" name="Bank Account Name" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{339A33EF-F310-4C33-9BA2-332E1474123E}" name="Bank Acc No" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{F29665B5-4DF1-44E7-A75D-FA717340214F}" name="Subtotal" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{FDD10ED1-DF47-4EC9-AB01-6CA58993EF2F}" name="Total" dataDxfId="1"/>
-    <tableColumn id="27" xr3:uid="{C4CF3119-1363-46DD-BD38-7474CA48138A}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{BC2DEE58-FEE2-4400-BFEB-FCEEFF738484}" name="Date" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{84C745BF-B192-406E-AE73-23BE614ABC77}" name="From" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{89ED4BCB-625D-483C-B61D-6C9F06C072FA}" name="Bill To" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{CE912894-973C-4E51-8011-D159986817C4}" name="Senders Address" dataDxfId="23"/>
+    <tableColumn id="24" xr3:uid="{BFE0D837-2C7B-42BD-A16A-DE2CDBF70628}" name="Receivers Address" dataDxfId="22"/>
+    <tableColumn id="25" xr3:uid="{62DFD726-84D8-495B-B42E-E0A59D973768}" name="Senders Contact Details" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{FE59F13E-5A21-47B4-A9EF-18DBAA382ABB}" name="Receivers Contact Details" dataDxfId="20"/>
+    <tableColumn id="28" xr3:uid="{B1D12C98-53A9-400A-90EC-3EC534830FE4}" name="Email" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{87932FF1-0A86-4F0D-9602-C05A18D4337E}" name="Inv No" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{E40660D4-E7F8-4155-BD74-B6079C1EDCB6}" name="Company Vat Reg" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{8E7E6CC3-BCDD-4C4B-AE2F-07C463573FBF}" name="PO No" dataDxfId="16"/>
+    <tableColumn id="23" xr3:uid="{02626E26-D8EF-44B0-9AB4-895DB15E6BAB}" name="VAT No" dataDxfId="15"/>
+    <tableColumn id="29" xr3:uid="{654A534F-1146-4C55-A284-5C0B5CAF3EB9}" name="VAT %" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{D979257E-475F-4CA9-A983-95369870AF9D}" name="Tax No" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{FA249B09-9B2D-4876-8E59-CF7C27DC3832}" name="Description" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{666804AA-1E70-415B-89D1-1A72FAF9F8EB}" name="Service" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{6EC2B118-0451-4EFE-8069-C6E9C3A002C0}" name="Qauntity" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{C05DC58D-14E4-40D2-BE25-405FE840F8AC}" name="Hours" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{C72C2D26-2E38-475A-AE9C-C967A09FC87E}" name="Rate" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{81F48D24-5ACC-4191-A21B-F84B9B5D0FE4}" name="Unit Price" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{634EBF08-2050-471F-A18B-0D975BEC91DC}" name="Price" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{038F4464-83DE-47BF-AAB6-6254BAA84B77}" name="Bank Name" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{BF7433D6-9279-442F-9D38-4A62C589F8B4}" name="Branch Code" dataDxfId="4"/>
+    <tableColumn id="26" xr3:uid="{B315133D-A01C-4DE4-A4C9-E0FC9A971EA0}" name="Bank Account Name" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{339A33EF-F310-4C33-9BA2-332E1474123E}" name="Bank Acc No" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{F29665B5-4DF1-44E7-A75D-FA717340214F}" name="Subtotal" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{FDD10ED1-DF47-4EC9-AB01-6CA58993EF2F}" name="Total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -679,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B17B189-3F58-460C-B125-67DE3543A8D8}">
-  <dimension ref="A1:AC14"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="B2:AB2"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1:AC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,7 +682,7 @@
     <col min="27" max="28" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -789,89 +767,83 @@
       <c r="AB1" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f t="shared" ref="A2:A14" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>45000</v>
+        <v>44437</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="1">
-        <v>199549990</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1234567</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
-      <c r="U2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" s="1"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Z2" s="1">
+        <v>859834000370</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>4228653</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>554002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4">
+        <v>45540</v>
+      </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="J3" s="1">
+        <v>2768710</v>
+      </c>
+      <c r="K3" s="1">
+        <v>47992</v>
+      </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -887,11 +859,14 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-      <c r="AC3" s="1"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA3" s="3">
+        <v>2230</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>2664.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -923,9 +898,8 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
-      <c r="AC4" s="1"/>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -957,9 +931,8 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
-      <c r="AC5" s="1"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -991,9 +964,8 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
-      <c r="AC6" s="1"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1025,9 +997,8 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
-      <c r="AC7" s="1"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1059,9 +1030,8 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
-      <c r="AC8" s="1"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1093,9 +1063,8 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
-      <c r="AC9" s="1"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1127,9 +1096,8 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
-      <c r="AC10" s="1"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1161,9 +1129,8 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
-      <c r="AC11" s="1"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1195,9 +1162,8 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
-      <c r="AC12" s="1"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1229,9 +1195,8 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
-      <c r="AC13" s="1"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1263,7 +1228,6 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
-      <c r="AC14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>